<commit_message>
Added code to assignment
</commit_message>
<xml_diff>
--- a/LaborStatistics Database Table Relationships.xlsx
+++ b/LaborStatistics Database Table Relationships.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="60">
   <si>
     <t>annual_2016</t>
   </si>
@@ -142,20 +142,80 @@
     <t>supersectore_name</t>
   </si>
   <si>
-    <t>`</t>
+    <t>x</t>
+  </si>
+  <si>
+    <t>-- SELECT i.industry_name</t>
+  </si>
+  <si>
+    <t>-- FROM industry as i </t>
+  </si>
+  <si>
+    <t>-- INNER JOIN series as s </t>
+  </si>
+  <si>
+    <t>-- ON i.industry_code = s.industry_code</t>
+  </si>
+  <si>
+    <t>-- SELECT MAX(j.value) as "Highest Average Weekly Hours Industry", MIN(j.value) as "Lowest Average Weekly Hours Industry", i.industry_name</t>
+  </si>
+  <si>
+    <t>-- JOIN series as s </t>
+  </si>
+  <si>
+    <t>-- JOIN january_2017 as j </t>
+  </si>
+  <si>
+    <t>-- ON j.series_id = s.series_id</t>
+  </si>
+  <si>
+    <t>-- FROM january_2017 as j</t>
+  </si>
+  <si>
+    <t>-- ON j.series_id = s.series_id </t>
+  </si>
+  <si>
+    <t>-- INNER JOIN datatype as d </t>
+  </si>
+  <si>
+    <t>-- ON d.data_type_code = s.data_type_code </t>
+  </si>
+  <si>
+    <t>-- INNER JOIN industry as i </t>
+  </si>
+  <si>
+    <t>-- WHERE j.series_id IN (SELECT s.series_id from series as s WHERE s.data_type_code IN </t>
+  </si>
+  <si>
+    <t>-- (SELECT d.data_type_code from datatype as d WHERE d.data_type_text = 'Average weekly hours of production and nonsupervisory employees'))</t>
+  </si>
+  <si>
+    <t>-- GROUP BY i.industry_name</t>
+  </si>
+  <si>
+    <t>-- ORDER BY MAX(j.value) ASC</t>
+  </si>
+  <si>
+    <t>-- HAVING MAX(j.value), MIN(j.value)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF008000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="12">
@@ -337,7 +397,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -356,6 +416,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1368,10 +1429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="E2:Q30"/>
+  <dimension ref="E2:Q57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N30" sqref="N30"/>
+      <selection activeCell="I42" sqref="I42:I57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1394,11 +1455,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="5:17">
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="13"/>
-      <c r="G2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="15"/>
     </row>
     <row r="3" spans="5:17">
       <c r="E3" s="4" t="s">
@@ -1408,11 +1469,11 @@
         <v>17</v>
       </c>
       <c r="G3" s="6"/>
-      <c r="L3" s="24" t="s">
+      <c r="L3" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="M3" s="25"/>
-      <c r="N3" s="26"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="27"/>
     </row>
     <row r="4" spans="5:17">
       <c r="E4" s="4" t="s">
@@ -1440,23 +1501,23 @@
       <c r="N5" s="6"/>
     </row>
     <row r="6" spans="5:17">
-      <c r="O6" s="27" t="s">
+      <c r="O6" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="P6" s="28"/>
-      <c r="Q6" s="29"/>
+      <c r="P6" s="29"/>
+      <c r="Q6" s="30"/>
     </row>
     <row r="7" spans="5:17">
-      <c r="E7" s="33" t="s">
+      <c r="E7" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="34"/>
-      <c r="G7" s="35"/>
-      <c r="I7" s="18" t="s">
+      <c r="F7" s="35"/>
+      <c r="G7" s="36"/>
+      <c r="I7" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="J7" s="19"/>
-      <c r="K7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="21"/>
       <c r="O7" s="4" t="s">
         <v>1</v>
       </c>
@@ -1589,21 +1650,21 @@
       <c r="Q14" s="6"/>
     </row>
     <row r="16" spans="5:17">
-      <c r="E16" s="30" t="s">
+      <c r="E16" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="F16" s="31"/>
-      <c r="G16" s="32"/>
-      <c r="I16" s="36" t="s">
+      <c r="F16" s="32"/>
+      <c r="G16" s="33"/>
+      <c r="I16" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="J16" s="37"/>
-      <c r="K16" s="38"/>
-      <c r="M16" s="21" t="s">
+      <c r="J16" s="38"/>
+      <c r="K16" s="39"/>
+      <c r="M16" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="N16" s="22"/>
-      <c r="O16" s="23"/>
+      <c r="N16" s="23"/>
+      <c r="O16" s="24"/>
     </row>
     <row r="17" spans="5:15">
       <c r="E17" s="4" t="s">
@@ -1704,11 +1765,11 @@
         <v>11</v>
       </c>
       <c r="G21" s="6"/>
-      <c r="I21" s="15" t="s">
+      <c r="I21" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="J21" s="16"/>
-      <c r="K21" s="17"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="18"/>
       <c r="M21" s="4" t="s">
         <v>5</v>
       </c>
@@ -1763,9 +1824,137 @@
       </c>
       <c r="O23" s="8"/>
     </row>
+    <row r="27" spans="5:15">
+      <c r="I27" s="12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="5:15">
+      <c r="I28" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="5:15">
+      <c r="I29" s="12" t="s">
+        <v>44</v>
+      </c>
+    </row>
     <row r="30" spans="5:15">
+      <c r="I30" s="12" t="s">
+        <v>45</v>
+      </c>
       <c r="N30" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="5:15">
+      <c r="I31" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="5:15">
+      <c r="I32" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="9:9">
+      <c r="I33" s="12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="9:9">
+      <c r="I34" s="12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="9:9">
+      <c r="I35" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="36" spans="9:9">
+      <c r="I36" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="42" spans="9:9">
+      <c r="I42" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="9:9">
+      <c r="I43" s="12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" spans="9:9">
+      <c r="I44" s="12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="9:9">
+      <c r="I45" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="46" spans="9:9">
+      <c r="I46" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="47" spans="9:9">
+      <c r="I47" s="12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="48" spans="9:9">
+      <c r="I48" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="49" spans="9:9">
+      <c r="I49" s="12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="50" spans="9:9">
+      <c r="I50" s="12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="51" spans="9:9">
+      <c r="I51" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="52" spans="9:9">
+      <c r="I52" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="53" spans="9:9">
+      <c r="I53" s="12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="54" spans="9:9">
+      <c r="I54" s="12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="55" spans="9:9">
+      <c r="I55" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="56" spans="9:9">
+      <c r="I56" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="57" spans="9:9">
+      <c r="I57" s="12" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>